<commit_message>
Website Add Login By Google Account and add section Data KTP in KYC Verification
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CRM_UserAccessManagement.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CRM_UserAccessManagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18650" windowHeight="7110" activeTab="1"/>
+    <workbookView windowWidth="17930" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>SearchUsername</t>
   </si>
@@ -41,52 +41,79 @@
     <t>RoleAccess</t>
   </si>
   <si>
-    <t>pricilia</t>
-  </si>
-  <si>
-    <t>Pricilia Agraria</t>
-  </si>
-  <si>
-    <t>pricial.agfaria@amarbank.co.id</t>
+    <t>Calistua Brigwitta</t>
+  </si>
+  <si>
+    <t>caliystaw</t>
+  </si>
+  <si>
+    <t>calista.rtta@amarbank.co.id</t>
   </si>
   <si>
     <t>Credit Admin</t>
   </si>
   <si>
-    <t>Pricilia123</t>
+    <t>Calista12334</t>
+  </si>
+  <si>
+    <t>apaya</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaa</t>
+  </si>
+  <si>
+    <t>caliystaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaa</t>
+  </si>
+  <si>
+    <t>calista.brigittta@amarbank.co.id</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Calista1234</t>
+  </si>
+  <si>
+    <t>AdminAll</t>
+  </si>
+  <si>
+    <t>caliystaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaaa</t>
+  </si>
+  <si>
+    <t>Calista1235</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>vrita</t>
-  </si>
-  <si>
-    <t>Vrita Esti</t>
-  </si>
-  <si>
-    <t>vrita.esti@amarbank.co.id</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Vrita12345</t>
-  </si>
-  <si>
-    <t>AdminAll</t>
-  </si>
-  <si>
-    <t>calista</t>
-  </si>
-  <si>
-    <t>Calista Brigitta</t>
-  </si>
-  <si>
-    <t>calista.brigitta@amarbank.co.id</t>
-  </si>
-  <si>
-    <t>Calista123</t>
+    <t>caliystaaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaaaa</t>
+  </si>
+  <si>
+    <t>Calista1236</t>
+  </si>
+  <si>
+    <t>videoproses</t>
+  </si>
+  <si>
+    <t>caliystaaaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigitttaaaaa</t>
+  </si>
+  <si>
+    <t>Calista1237</t>
+  </si>
+  <si>
+    <t>verificationlihat</t>
   </si>
 </sst>
 </file>
@@ -94,10 +121,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -110,19 +137,20 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,23 +158,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,9 +174,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,24 +204,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,9 +234,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,21 +265,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,6 +288,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -273,175 +318,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,6 +479,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -473,37 +520,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,12 +570,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -575,130 +602,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -706,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,13 +1055,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="11.1818181818182" customWidth="1"/>
@@ -1071,12 +1098,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -1096,42 +1126,45 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -1140,14 +1173,68 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pricial.agfaria@amarbank.co.id"/>
-    <hyperlink ref="D3" r:id="rId2" display="vrita.esti@amarbank.co.id"/>
-    <hyperlink ref="D4" r:id="rId3" display="calista.brigitta@amarbank.co.id"/>
+    <hyperlink ref="D3" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D4" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D2" r:id="rId2" display="calista.rtta@amarbank.co.id" tooltip="mailto:calista.rtta@amarbank.co.id"/>
+    <hyperlink ref="D5" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D6" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1157,21 +1244,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="11.1818181818182" customWidth="1"/>
-    <col min="3" max="3" width="13.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="19.6363636363636" customWidth="1"/>
     <col min="4" max="4" width="29.1818181818182" customWidth="1"/>
     <col min="5" max="6" width="14.7272727272727" customWidth="1"/>
     <col min="7" max="7" width="16.0909090909091" customWidth="1"/>
-    <col min="8" max="8" width="12.2727272727273" customWidth="1"/>
+    <col min="8" max="8" width="17.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1200,12 +1287,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -1225,42 +1315,45 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -1269,14 +1362,68 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pricial.agfaria@amarbank.co.id"/>
-    <hyperlink ref="D3" r:id="rId2" display="vrita.esti@amarbank.co.id"/>
-    <hyperlink ref="D4" r:id="rId3" display="calista.brigitta@amarbank.co.id"/>
+    <hyperlink ref="D3" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D4" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D2" r:id="rId2" display="calista.rtta@amarbank.co.id" tooltip="mailto:calista.rtta@amarbank.co.id"/>
+    <hyperlink ref="D5" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D6" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Website-leadsmanagement(backToBucketList, ChangeIntoPending, DetailsHarusDitelpon, DetailsPending, DetailsReject, PageNotFound, Pagination, URLWithID)
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CRM_UserAccessManagement.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CRM_UserAccessManagement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18650" windowHeight="7110" activeTab="1"/>
+    <workbookView windowWidth="17930" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="Development" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>SearchUsername</t>
   </si>
@@ -41,52 +41,79 @@
     <t>RoleAccess</t>
   </si>
   <si>
-    <t>pricilia</t>
-  </si>
-  <si>
-    <t>Pricilia Agraria</t>
-  </si>
-  <si>
-    <t>pricial.agfaria@amarbank.co.id</t>
+    <t>Calistua Brigwitta</t>
+  </si>
+  <si>
+    <t>caliystaw</t>
+  </si>
+  <si>
+    <t>calista.rtta@amarbank.co.id</t>
   </si>
   <si>
     <t>Credit Admin</t>
   </si>
   <si>
-    <t>Pricilia123</t>
+    <t>Calista12334</t>
+  </si>
+  <si>
+    <t>apaya</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaa</t>
+  </si>
+  <si>
+    <t>caliystaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaa</t>
+  </si>
+  <si>
+    <t>calista.brigittta@amarbank.co.id</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Calista1234</t>
+  </si>
+  <si>
+    <t>AdminAll</t>
+  </si>
+  <si>
+    <t>caliystaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaaa</t>
+  </si>
+  <si>
+    <t>Calista1235</t>
   </si>
   <si>
     <t>Admin</t>
   </si>
   <si>
-    <t>vrita</t>
-  </si>
-  <si>
-    <t>Vrita Esti</t>
-  </si>
-  <si>
-    <t>vrita.esti@amarbank.co.id</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Vrita12345</t>
-  </si>
-  <si>
-    <t>AdminAll</t>
-  </si>
-  <si>
-    <t>calista</t>
-  </si>
-  <si>
-    <t>Calista Brigitta</t>
-  </si>
-  <si>
-    <t>calista.brigitta@amarbank.co.id</t>
-  </si>
-  <si>
-    <t>Calista123</t>
+    <t>caliystaaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigittaaaaa</t>
+  </si>
+  <si>
+    <t>Calista1236</t>
+  </si>
+  <si>
+    <t>videoproses</t>
+  </si>
+  <si>
+    <t>caliystaaaaa</t>
+  </si>
+  <si>
+    <t>Calistua Brigitttaaaaa</t>
+  </si>
+  <si>
+    <t>Calista1237</t>
+  </si>
+  <si>
+    <t>verificationlihat</t>
   </si>
 </sst>
 </file>
@@ -94,10 +121,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -110,19 +137,20 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -130,23 +158,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,9 +174,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,24 +204,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,9 +234,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,21 +265,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,6 +288,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -273,175 +318,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,6 +479,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -473,37 +520,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -552,12 +570,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -575,130 +602,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -706,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1028,13 +1055,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="$A1:$XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="11.1818181818182" customWidth="1"/>
@@ -1071,12 +1098,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -1096,42 +1126,45 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -1140,14 +1173,68 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pricial.agfaria@amarbank.co.id"/>
-    <hyperlink ref="D3" r:id="rId2" display="vrita.esti@amarbank.co.id"/>
-    <hyperlink ref="D4" r:id="rId3" display="calista.brigitta@amarbank.co.id"/>
+    <hyperlink ref="D3" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D4" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D2" r:id="rId2" display="calista.rtta@amarbank.co.id" tooltip="mailto:calista.rtta@amarbank.co.id"/>
+    <hyperlink ref="D5" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D6" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1157,21 +1244,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="17.9090909090909" customWidth="1"/>
     <col min="2" max="2" width="11.1818181818182" customWidth="1"/>
-    <col min="3" max="3" width="13.2727272727273" customWidth="1"/>
+    <col min="3" max="3" width="19.6363636363636" customWidth="1"/>
     <col min="4" max="4" width="29.1818181818182" customWidth="1"/>
     <col min="5" max="6" width="14.7272727272727" customWidth="1"/>
     <col min="7" max="7" width="16.0909090909091" customWidth="1"/>
-    <col min="8" max="8" width="12.2727272727273" customWidth="1"/>
+    <col min="8" max="8" width="17.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1200,12 +1287,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -1225,42 +1315,45 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>23</v>
@@ -1269,14 +1362,68 @@
         <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="pricial.agfaria@amarbank.co.id"/>
-    <hyperlink ref="D3" r:id="rId2" display="vrita.esti@amarbank.co.id"/>
-    <hyperlink ref="D4" r:id="rId3" display="calista.brigitta@amarbank.co.id"/>
+    <hyperlink ref="D3" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D4" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D2" r:id="rId2" display="calista.rtta@amarbank.co.id" tooltip="mailto:calista.rtta@amarbank.co.id"/>
+    <hyperlink ref="D5" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
+    <hyperlink ref="D6" r:id="rId1" display="calista.brigittta@amarbank.co.id" tooltip="mailto:calista.brigittta@amarbank.co.id"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>